<commit_message>
core: reg: Add register set and simple isim test
Signed-off-by: Ben Lancaster <bdl@live.co.uk>
</commit_message>
<xml_diff>
--- a/doc/gantt/gantt.xlsx
+++ b/doc/gantt/gantt.xlsx
@@ -1406,8 +1406,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="0" y="2152651"/>
-          <a:ext cx="9819489" cy="1895475"/>
+          <a:off x="0" y="2152664"/>
+          <a:ext cx="9819501" cy="1895451"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -1907,11 +1907,11 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.32294</cdr:x>
+      <cdr:x>0.3173</cdr:x>
       <cdr:y>0</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.333</cdr:x>
+      <cdr:x>0.32736</cdr:x>
       <cdr:y>1</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
@@ -1927,8 +1927,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="3057526" y="0"/>
-          <a:ext cx="95250" cy="5086350"/>
+          <a:off x="3212642" y="0"/>
+          <a:ext cx="101858" cy="6086475"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -2420,7 +2420,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>